<commit_message>
add ft/s for line velocity
</commit_message>
<xml_diff>
--- a/PSP Pathfinder Line Velocity.xlsx
+++ b/PSP Pathfinder Line Velocity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://purdue0-my.sharepoint.com/personal/jmedasan_purdue_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\PSPL_Rocket_A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{404B236B-E779-4805-A57B-F80687362D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B332EF-DD6A-4042-958B-46303FD48067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Tube Sizes</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t xml:space="preserve">Density of IPA </t>
+  </si>
+  <si>
+    <t>Oxidizer Line Velocity (ft/s)</t>
+  </si>
+  <si>
+    <t>Fuel Line Velocity (ft/s)</t>
   </si>
 </sst>
 </file>
@@ -144,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -158,6 +164,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,24 +386,28 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="25.77734375" customWidth="1"/>
-    <col min="3" max="3" width="21.21875" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.26953125" customWidth="1"/>
+    <col min="3" max="3" width="28.6328125" customWidth="1"/>
+    <col min="4" max="4" width="21.36328125" customWidth="1"/>
+    <col min="6" max="6" width="26.26953125" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -406,8 +420,14 @@
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0.25</v>
       </c>
@@ -422,8 +442,16 @@
         <f t="shared" ref="D3:D9" si="1">$B$16/((3.14*(A3*0.0254)^2)/4)</f>
         <v>32.452318916728402</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="8">
+        <f>C3*3.28084</f>
+        <v>73.344522937669353</v>
+      </c>
+      <c r="G3" s="8">
+        <f>D3*3.28084</f>
+        <v>106.47086599475921</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0.375</v>
       </c>
@@ -438,8 +466,16 @@
         <f t="shared" si="1"/>
         <v>14.42325285187929</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="8">
+        <f t="shared" ref="F4:F9" si="2">C4*3.28084</f>
+        <v>32.597565750075269</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" ref="G4:G9" si="3">D4*3.28084</f>
+        <v>47.320384886559651</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>0.5</v>
       </c>
@@ -454,8 +490,16 @@
         <f t="shared" si="1"/>
         <v>8.1130797291821004</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="8">
+        <f t="shared" si="2"/>
+        <v>18.336130734417338</v>
+      </c>
+      <c r="G5" s="8">
+        <f t="shared" si="3"/>
+        <v>26.617716498689802</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>0.625</v>
       </c>
@@ -470,8 +514,16 @@
         <f t="shared" si="1"/>
         <v>5.1923710266765433</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="8">
+        <f t="shared" si="2"/>
+        <v>11.735123670027093</v>
+      </c>
+      <c r="G6" s="8">
+        <f t="shared" si="3"/>
+        <v>17.03533855916147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>0.75</v>
       </c>
@@ -486,8 +538,16 @@
         <f t="shared" si="1"/>
         <v>3.6058132129698226</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="8">
+        <f t="shared" si="2"/>
+        <v>8.1493914375188172</v>
+      </c>
+      <c r="G7" s="8">
+        <f t="shared" si="3"/>
+        <v>11.830096221639913</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -502,8 +562,16 @@
         <f t="shared" si="1"/>
         <v>2.0282699322955251</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="8">
+        <f t="shared" si="2"/>
+        <v>4.5840326836043346</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" si="3"/>
+        <v>6.6544291246724505</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1.5</v>
       </c>
@@ -518,8 +586,19 @@
         <f t="shared" si="1"/>
         <v>0.90145330324245565</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="8">
+        <f t="shared" si="2"/>
+        <v>2.0373478593797043</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" si="3"/>
+        <v>2.9575240554099782</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -530,7 +609,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -541,15 +620,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="2">
-        <f t="shared" ref="B15:B16" si="2">(B12*0.453592)/D15</f>
+        <f t="shared" ref="B15:B16" si="4">(B12*0.453592)/D15</f>
         <v>7.0761942156003497E-4</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -562,12 +641,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.027218524173028E-3</v>
       </c>
       <c r="C16" s="2" t="s">

</xml_diff>